<commit_message>
adiciona funções e melhora funcionalidades
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\Envia E_mail\Envia_Email\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\Envia_Email\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6536DB3-DB22-4E65-BC7C-DA9ACA0F6345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3DA4C1-1104-4462-BFF9-54D445539048}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{028B4A53-2451-43C6-9918-8740B5B31A80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Nome</t>
   </si>
@@ -33,34 +33,20 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Caio Padovani Costa</t>
+    <t>Status</t>
   </si>
   <si>
-    <t>caiocosta8@hotmail.com</t>
-  </si>
-  <si>
-    <t>Eliana Costa Martins</t>
-  </si>
-  <si>
-    <t>elicmartins@gmail.com</t>
+    <t>Data Envio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,16 +69,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,41 +390,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B9E81E-288C-4ADF-BA25-5651D4F86D8D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
corrige envio de assinatura por imagem
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\Envia_Email\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3DA4C1-1104-4462-BFF9-54D445539048}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB09579-38BD-4EAE-88A5-887283E4A891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{028B4A53-2451-43C6-9918-8740B5B31A80}"/>
   </bookViews>
@@ -72,10 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,9 +388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B9E81E-288C-4ADF-BA25-5651D4F86D8D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -416,17 +416,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>